<commit_message>
Update template cho tài liệu change request form
</commit_message>
<xml_diff>
--- a/1. Project management/5. Change management plan/AS_PM_ChangeRequestFor_Template.xlsx
+++ b/1. Project management/5. Change management plan/AS_PM_ChangeRequestFor_Template.xlsx
@@ -183,14 +183,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -472,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,6 +506,111 @@
     <xf numFmtId="14" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -515,117 +620,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -660,6 +654,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,14 +750,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>428625</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1781175</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>400050</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -807,7 +810,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -830,14 +833,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>2219325</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>3571875</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>390525</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -890,7 +893,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -913,14 +916,14 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>4019550</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>5372100</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>400050</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -973,7 +976,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1000,15 +1003,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>323850</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1390650</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1061,7 +1064,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1084,14 +1087,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>1285875</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1144,7 +1147,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1166,15 +1169,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>723900</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:colOff>742950</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1227,7 +1230,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1250,14 +1253,14 @@
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>1066800</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1310,7 +1313,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1332,15 +1335,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>314325</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1266825</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1393,7 +1396,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1415,15 +1418,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1219200</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:colOff>1123950</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1476,7 +1479,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1498,15 +1501,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>390525</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:colOff>209550</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1559,7 +1562,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1581,15 +1584,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:colOff>1066800</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1642,7 +1645,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1664,15 +1667,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1266825</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:colOff>1276350</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1725,7 +1728,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1747,15 +1750,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>1266825</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>295275</xdr:rowOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1808,7 +1811,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1835,15 +1838,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>762000</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1009650</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:colOff>304800</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1896,7 +1899,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1918,15 +1921,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>457200</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>409575</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>266700</xdr:rowOff>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1979,7 +1982,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="vi-VN" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2286,29 +2289,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.875" customWidth="1"/>
-    <col min="2" max="2" width="86" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="114.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
@@ -2340,7 +2343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -2348,7 +2351,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>41</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2364,7 +2367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
@@ -2380,14 +2383,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
@@ -2407,14 +2408,14 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>428625</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1781175</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>400050</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2429,14 +2430,14 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>2219325</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>3571875</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>390525</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2451,14 +2452,14 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4019550</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>5372100</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>400050</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2476,65 +2477,65 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.375" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-    </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-    </row>
-    <row r="5" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-    </row>
-    <row r="6" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -2544,116 +2545,116 @@
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-    </row>
-    <row r="9" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
-    </row>
-    <row r="12" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="24" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2688,15 +2689,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>323850</xdr:rowOff>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1390650</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2711,14 +2712,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>57150</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>1285875</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2732,15 +2733,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>723900</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:colOff>742950</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2755,14 +2756,14 @@
                   <from>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>1066800</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2776,15 +2777,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>485775</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>314325</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1266825</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2798,15 +2799,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1219200</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:colOff>1123950</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2820,15 +2821,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>390525</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>533400</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:colOff>209550</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2842,15 +2843,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:colOff>1066800</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2864,15 +2865,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1266825</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:colOff>1276350</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2886,15 +2887,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>1266825</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>295275</xdr:rowOff>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2912,94 +2913,94 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.625" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="42.625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="52"/>
-    </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="46"/>
-    </row>
-    <row r="9" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="18" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="A1:E1"/>
@@ -3007,6 +3008,7 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3017,27 +3019,27 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.25" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
@@ -3048,79 +3050,79 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-    </row>
-    <row r="5" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
-    </row>
-    <row r="6" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
-    </row>
-    <row r="7" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
-    </row>
-    <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="56" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3148,15 +3150,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>762000</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>1009650</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:colOff>304800</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3170,15 +3172,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>457200</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>409575</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>266700</xdr:rowOff>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>